<commit_message>
Updates ETL cost objects in work orders
</commit_message>
<xml_diff>
--- a/Work Orders/ETL_blank_elec_workorder.xlsx
+++ b/Work Orders/ETL_blank_elec_workorder.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B8FDC8-F6F1-4D62-8285-4663812E7AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6225" windowWidth="19410" windowHeight="6150"/>
+    <workbookView xWindow="-25350" yWindow="4905" windowWidth="18510" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -113,9 +126,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Info:</t>
-  </si>
-  <si>
-    <t>26-0521-0189-001</t>
   </si>
   <si>
     <t>Frank Golf</t>
@@ -133,11 +143,14 @@
       <t>for ETL</t>
     </r>
   </si>
+  <si>
+    <t>26-0521-0189-002 M&amp;S -003 Labor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -848,6 +861,62 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -902,10 +971,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -918,60 +983,8 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1093,6 +1106,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2049"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1175,6 +1191,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1466,14 +1485,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="B4" sqref="B4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1493,7 +1512,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1506,15 +1525,15 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="62" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="63"/>
+      <c r="E2" s="77"/>
       <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
@@ -1522,24 +1541,24 @@
         <v>25</v>
       </c>
       <c r="H2" s="10"/>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="55"/>
+      <c r="J2" s="69"/>
     </row>
     <row r="3" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="64" t="s">
+      <c r="A3" s="73"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="81" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="78"/>
+      <c r="F3" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="66"/>
-      <c r="H3" s="67"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="80"/>
       <c r="I3" s="13"/>
       <c r="J3" s="14"/>
     </row>
@@ -1547,26 +1566,26 @@
       <c r="A4" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="50"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="64"/>
     </row>
     <row r="5" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="53"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="67"/>
       <c r="H5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1610,13 +1629,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="68"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="70"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="57"/>
       <c r="H7" s="31"/>
       <c r="I7" s="42"/>
       <c r="J7" s="20">
@@ -1625,13 +1644,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="71"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="70"/>
+      <c r="A8" s="61"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="57"/>
       <c r="H8" s="32"/>
       <c r="I8" s="43"/>
       <c r="J8" s="45">
@@ -1640,13 +1659,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="68"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="57"/>
       <c r="H9" s="31"/>
       <c r="I9" s="42"/>
       <c r="J9" s="20">
@@ -1655,13 +1674,13 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="71"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="70"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="32"/>
       <c r="I10" s="43"/>
       <c r="J10" s="45">
@@ -1670,13 +1689,13 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="68"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="70"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="31"/>
       <c r="I11" s="42"/>
       <c r="J11" s="20">
@@ -1685,13 +1704,13 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="71"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="70"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="57"/>
       <c r="H12" s="32"/>
       <c r="I12" s="43"/>
       <c r="J12" s="45">
@@ -1700,13 +1719,13 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="68"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="70"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="57"/>
       <c r="H13" s="31"/>
       <c r="I13" s="42"/>
       <c r="J13" s="20">
@@ -1715,13 +1734,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="71"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="70"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
       <c r="H14" s="32"/>
       <c r="I14" s="43"/>
       <c r="J14" s="45">
@@ -1730,15 +1749,15 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="70"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="57"/>
       <c r="H15" s="31"/>
       <c r="I15" s="42"/>
       <c r="J15" s="20">
@@ -1747,13 +1766,13 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="71"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="70"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="57"/>
       <c r="H16" s="32"/>
       <c r="I16" s="43"/>
       <c r="J16" s="45">
@@ -1762,13 +1781,13 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="68"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
       <c r="H17" s="31"/>
       <c r="I17" s="42"/>
       <c r="J17" s="20">
@@ -1853,291 +1872,291 @@
       <c r="A22" s="33"/>
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
-      <c r="D22" s="72" t="s">
+      <c r="D22" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="74"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="60"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="46"/>
       <c r="B23" s="35"/>
       <c r="C23" s="35"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="77"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="50"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="47"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="76"/>
-      <c r="J24" s="77"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="50"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="46"/>
       <c r="B25" s="35"/>
       <c r="C25" s="35"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="77"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="50"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="47"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="76"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="76"/>
-      <c r="I26" s="76"/>
-      <c r="J26" s="77"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="50"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="46"/>
       <c r="B27" s="35"/>
       <c r="C27" s="35"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="77"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="50"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="47"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="76"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="77"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="46"/>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="77"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="47"/>
       <c r="B30" s="36"/>
       <c r="C30" s="36"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="77"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="50"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="46"/>
       <c r="B31" s="35"/>
       <c r="C31" s="35"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="76"/>
-      <c r="I31" s="76"/>
-      <c r="J31" s="77"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="50"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="47"/>
       <c r="B32" s="36"/>
       <c r="C32" s="36"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="76"/>
-      <c r="H32" s="76"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="77"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="50"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="46"/>
       <c r="B33" s="35"/>
       <c r="C33" s="35"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="76"/>
-      <c r="J33" s="77"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="50"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="47"/>
       <c r="B34" s="36"/>
       <c r="C34" s="36"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
-      <c r="G34" s="76"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="77"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="50"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="46"/>
       <c r="B35" s="35"/>
       <c r="C35" s="35"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="77"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="50"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="47"/>
       <c r="B36" s="36"/>
       <c r="C36" s="36"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="77"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="50"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="46"/>
       <c r="B37" s="35"/>
       <c r="C37" s="35"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="76"/>
-      <c r="J37" s="77"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="50"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="47"/>
       <c r="B38" s="36"/>
       <c r="C38" s="36"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="76"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="76"/>
-      <c r="H38" s="76"/>
-      <c r="I38" s="76"/>
-      <c r="J38" s="77"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="50"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="46"/>
       <c r="B39" s="35"/>
       <c r="C39" s="35"/>
-      <c r="D39" s="75"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="77"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="50"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="47"/>
       <c r="B40" s="36"/>
       <c r="C40" s="36"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="76"/>
-      <c r="J40" s="77"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="50"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="46"/>
       <c r="B41" s="35"/>
       <c r="C41" s="35"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
-      <c r="J41" s="77"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="50"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="47"/>
       <c r="B42" s="36"/>
       <c r="C42" s="36"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="76"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="76"/>
-      <c r="J42" s="77"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="46"/>
       <c r="B43" s="35"/>
       <c r="C43" s="35"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="76"/>
-      <c r="J43" s="77"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="50"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="47"/>
       <c r="B44" s="36"/>
       <c r="C44" s="36"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="76"/>
-      <c r="G44" s="76"/>
-      <c r="H44" s="76"/>
-      <c r="I44" s="76"/>
-      <c r="J44" s="77"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="50"/>
     </row>
     <row r="45" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="46"/>
       <c r="B45" s="35"/>
       <c r="C45" s="35"/>
-      <c r="D45" s="79"/>
-      <c r="E45" s="80"/>
-      <c r="F45" s="80"/>
-      <c r="G45" s="80"/>
-      <c r="H45" s="80"/>
-      <c r="I45" s="80"/>
-      <c r="J45" s="81"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="54"/>
     </row>
     <row r="46" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27" t="s">
@@ -2208,41 +2227,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="43">
-    <mergeCell ref="D41:J41"/>
-    <mergeCell ref="D42:J42"/>
-    <mergeCell ref="D43:J43"/>
-    <mergeCell ref="D44:J44"/>
-    <mergeCell ref="D45:J45"/>
-    <mergeCell ref="D36:J36"/>
-    <mergeCell ref="D37:J37"/>
-    <mergeCell ref="D38:J38"/>
-    <mergeCell ref="D39:J39"/>
-    <mergeCell ref="D40:J40"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="D32:J32"/>
-    <mergeCell ref="D33:J33"/>
-    <mergeCell ref="D34:J34"/>
-    <mergeCell ref="D35:J35"/>
-    <mergeCell ref="D26:J26"/>
-    <mergeCell ref="D27:J27"/>
-    <mergeCell ref="D28:J28"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="D30:J30"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="D22:J22"/>
-    <mergeCell ref="D23:J23"/>
-    <mergeCell ref="D24:J24"/>
-    <mergeCell ref="D25:J25"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A11:G11"/>
     <mergeCell ref="B4:J4"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="I2:J2"/>
@@ -2251,6 +2235,41 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="D24:J24"/>
+    <mergeCell ref="D25:J25"/>
+    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="D27:J27"/>
+    <mergeCell ref="D28:J28"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="D30:J30"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="D32:J32"/>
+    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="D34:J34"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="D36:J36"/>
+    <mergeCell ref="D37:J37"/>
+    <mergeCell ref="D38:J38"/>
+    <mergeCell ref="D39:J39"/>
+    <mergeCell ref="D40:J40"/>
+    <mergeCell ref="D41:J41"/>
+    <mergeCell ref="D42:J42"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="D44:J44"/>
+    <mergeCell ref="D45:J45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2310,6 +2329,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AD45A7EE92C7A8439247C65C4DDDB32C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0603451c8101eb4b7681b060238afd68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4f22facd-6011-4514-bb27-668268174520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89c41b19dc4dba1030c844a5b6ea91b3" ns3:_="">
     <xsd:import namespace="4f22facd-6011-4514-bb27-668268174520"/>
@@ -2493,35 +2527,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{796B72F4-EC46-4855-A84A-92C9152C4039}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8585D35B-7786-4FE5-9CA6-1108E4D8F830}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4f22facd-6011-4514-bb27-668268174520"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2543,9 +2552,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8585D35B-7786-4FE5-9CA6-1108E4D8F830}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{796B72F4-EC46-4855-A84A-92C9152C4039}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4f22facd-6011-4514-bb27-668268174520"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>